<commit_message>
Update exceptions for criteria evaluation
</commit_message>
<xml_diff>
--- a/post_criteria_evaluation.xlsx
+++ b/post_criteria_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,24 +573,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nafhan Najib</t>
+          <t>Kelvin Ee</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+60-127445518</t>
+          <t>+60 11-3919 0131</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>nafhannajib@gmail.com</t>
+          <t>kelvinee2001@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Region Leader', 'job_company': 'Foxconn Vietnam plant', 'Industries': ['Electronic Manufacturing', 'Technology', 'Electrical Equipment Manufacturing', 'Engineering and Construction'], 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'Kajang, Selangor', 'job_duration': 'N/A'}, {'job_title': 'Sony Green Partner Auditor', 'job_company': 'N/A', 'Industries': ['Unknown'], 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Electrical Model Leader', 'job_company': 'KIT Plant (Egypt)', 'Industries': ['Unknown'], 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Senior Design Engineer (Project)', 'job_company': 'Sony EMCS (M) Sdn Bhd', 'Industries': ['Electronics', 'Manufacturing', 'Technology', 'Consumer Electronics'], 'start_date': 'Dec 2018', 'end_date': 'Present', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Intern', 'job_company': 'AEM Microtronics Sdn Bhd', 'Industries': ['Unknown'], 'start_date': 'Feb 2018', 'end_date': 'Jun 2018', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Intern', 'job_company': 'Hospital Sultanah Bahiyah', 'Industries': ['Health Care', 'Public Administration'], 'start_date': 'Jul 2017', 'end_date': 'Aug 2017', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
+          <t>[{'job_title': 'PHP Web Developer', 'job_company': 'Powerec Services Sdn Bhd', 'Industries': ['Unknown'], 'start_date': '2021-11', 'end_date': '2022-02', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'PPG Intern', 'job_company': 'N/A', 'Industries': ['Unknown'], 'start_date': '2023-08', 'end_date': '2024-05-19 11:33:54.994675', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -600,38 +600,38 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Physics', 'level': 'Bachelor of Science', 'cgpa': '3.45', 'university': 'Universiti Sains Malaysia', 'start_date': '2015', 'year_of_graduation': '2018'}, {'field_of_study': 'Innovation &amp; Engineering Design', 'level': 'Master of Science', 'cgpa': '3.94', 'university': 'Universiti Putra Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
+          <t>[{'field_of_study': 'Bachelor of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.98', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': 'N/A'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['N/A']</t>
+          <t>['Alteryx Designer Core Certified']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Python', 'Visual Basic for Application (VBA)', 'C++', 'Microsoft Power BI', 'Solidworks', 'Applied Data Engineer', 'Google Project Management', 'Digital Leadership Development', 'Python 3 Programming']</t>
+          <t>['Python', 'SQL', 'C++', 'R', 'Power BI', 'Tableau', 'Alteryx', 'Excel', 'Databricks', 'Azure Data Factory', 'Blob Storage', 'KeyVault', 'HTML', 'CSS', 'PHP', 'Bootstrap', 'JavaScript', 'C#', 'Cloud Foundation', 'Machine Learning', 'Data Analytic']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Malay', 'English', 'Mandarin', 'Spanish']</t>
+          <t>['English', 'Malay', 'Chinese']</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M2" t="n">
-        <v>7</v>
+        <v>2.8</v>
       </c>
       <c r="N2" t="n">
-        <v>4.8</v>
+        <v>6.9</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="T2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -655,7 +655,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t xml:space="preserve">2020, 2018, </t>
+          <t xml:space="preserve">N/A, </t>
         </is>
       </c>
       <c r="X2" t="n">
@@ -667,142 +667,19 @@
       <c r="Z2" t="inlineStr">
         <is>
           <t>**Alignments:**
-1. **Education Background:**
-   - The candidate has a Bachelor's degree in Physics and a Master's degree in Innovation &amp; Engineering Design, which aligns with the job requirements that may require a strong educational background in science and engineering.
-2. **Skills:**
-   - The candidate possesses skills in Python, C++, and Microsoft Power BI, which are relevant to the job description that may involve data analysis and programming tasks.
-3. **Previous Job Roles:**
-   - The candidate has experience working in roles related to engineering, electronics, and technology, which aligns with the job description that may require experience in similar industries.
-4. **Languages:**
-   - The candidate is proficient in Malay, English, Mandarin, and Spanish, which could be beneficial for a role that involves communication with diverse teams or clients.
+- The candidate holds a Bachelor's Degree in Computer Science with a focus on Data Engineering, which aligns with the educational background required for the job.
+- The candidate has skills in Python, SQL, Power BI, Tableau, Alteryx, and other relevant tools and technologies mentioned in the job requirements.
+- The candidate has professional certification in Alteryx, which is a plus as Alteryx is mentioned in the job requirements.
+- The candidate is proficient in English, Malay, and Chinese languages, which can be beneficial for communication in a diverse work environment.
 **Misalignments:**
-1. **Professional Certificate:**
-   - The candidate does not have any professional certificates listed, which may be a misalignment if the job description specifically requires certain certifications.
-2. **Job Duration Details:**
-   - Some of the previous job roles listed have "N/A" for start date, end date, and job duration, which may make it difficult to assess the candidate's experience and tenure in those positions.
-3. **Industries in Previous Job Roles:**
-   - Some of the industries mentioned in the candidate's previous job roles are listed as "Unknown," which may not provide clear insight into the candidate's experience in those specific industries.
-Overall, the candidate's educational background, skills, and experience align well with the job description, but there are some misalignments in terms of professional certificates, job duration details, and clarity on industries worked in.</t>
+- The candidate's previous job roles as a PHP Web Developer and PPG Intern do not directly align with the job description for a Data Engineer.
+- The candidate's previous job roles do not demonstrate direct experience in data engineering or related fields.
+- The candidate's previous job roles do not show experience with the specific tools and technologies mentioned in the job requirements, such as Azure Data Factory, Blob Storage, and Databricks.
+- The candidate's previous job roles do not indicate experience with machine learning or data analytics, which are mentioned in the job requirements.</t>
         </is>
       </c>
       <c r="AA2" t="n">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>NURUL SHAHIRAH BINTI MOHD IDRIS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+6013 3872826</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>shahirahidris98@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[{'job_title': 'Market Research Analyst', 'job_company': 'MANPOWER GROUP MALAYSIA', 'Industries': ['Human Resources', 'Employment Services'], 'start_date': '2022-05', 'end_date': '2022-09', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'R&amp;D and QC Chemist', 'job_company': 'SMART INK SDN BHD', 'Industries': ['Unknown'], 'start_date': '2021-04', 'end_date': '2022-04', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Research Assistant Intern', 'job_company': 'UNIVERSITI PUTRA MALAYSIA', 'Industries': ['Education'], 'start_date': '2019-06', 'end_date': '2019-09', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>[{'Country': 'N/A', 'State': 'N/A', 'City': 'N/A'}]</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[{'field_of_study': 'Applied Chemistry', 'level': "Bachelor's", 'cgpa': 'N/A', 'university': 'Universiti Teknologi MARA', 'start_date': '2017', 'year_of_graduation': '2021'}]</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>['Zero Microsoft Excel Complete 2020', 'Google Data Analytics', 'Data Star Program Data Analyst']</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>['Microsoft Word', 'Microsoft Excel', 'Microsoft PowerPoint', 'C++ Programming Language', 'Microsoft Outlook', 'ChemDraw', 'Microsoft Access', 'Python Programming Language', 'SQL', 'Tableau']</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>['Bahasa Melayu', 'English', 'Bahasa Indonesia', 'Japanese', 'Arabic']</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="N3" t="n">
-        <v>4.65</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>5</v>
-      </c>
-      <c r="T3" t="n">
-        <v>8</v>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>No exact match and no matching industry from past employers detected</t>
-        </is>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2021, </t>
-        </is>
-      </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>**Alignments:**
-- The candidate has a Bachelor's degree in Applied Chemistry, which aligns with the job requirement of a background in chemistry.
-- The candidate has skills in Microsoft Excel, Microsoft PowerPoint, Python Programming Language, and SQL, which are relevant to the job requirements.
-- The candidate has previous job experience as an R&amp;D and QC Chemist, which aligns with the job description of a chemist role.
-- The candidate has professional certificates in Data Analytics and Data Analyst, which are relevant to the job requirements.
-- The candidate is proficient in English, which is required for the job.
-**Misalignments:**
-- The candidate's previous job roles are not directly related to the specific industry mentioned in the job description.
-- The candidate's language skills in Bahasa Melayu, Bahasa Indonesia, Japanese, and Arabic may not be directly relevant to the job requirements unless specified.
-- The candidate's skill in C++ Programming Language and ChemDraw are not mentioned in the job requirements.</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>21.45</v>
+        <v>28.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update format education background
</commit_message>
<xml_diff>
--- a/post_criteria_evaluation.xlsx
+++ b/post_criteria_evaluation.xlsx
@@ -573,24 +573,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Kelvin Ee</t>
+          <t>ANG YI LING</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+60 11-3919 0131</t>
+          <t>014-6263882</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>kelvinee2001@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>yi_ling13@hotmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'PHP Web Developer', 'job_company': 'Powerec Services Sdn Bhd', 'Industries': ['Unknown'], 'start_date': '2021-11', 'end_date': '2022-02', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'PPG Intern', 'job_company': 'N/A', 'Industries': ['Unknown'], 'start_date': '2023-08', 'end_date': '2024-05-19 11:33:54.994675', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
+          <t>[{'job_title': 'SENIOR CORPORATE TRAVEL CONSULTANT', 'job_company': 'FCM TRAVEL SOLUTIONS MALAYSIA', 'Industries': ['Travel and Tourism'], 'start_date': '2018-11', 'end_date': '2021-07', 'job_location': 'Malaysia', 'job_duration': '2 years 9 months'}, {'job_title': 'SENIOR CORPORATE TRAVEL CONSULTANT', 'job_company': 'FCM TRAVEL SINGAPORE', 'Industries': ['Travel and Tourism'], 'start_date': '2021-08', 'end_date': '2021-11', 'job_location': 'Singapore', 'job_duration': '3 months'}, {'job_title': 'CORPORATE TRAVEL CONSULTANT', 'job_company': 'HOLIDAY TOURS SDN BHD', 'Industries': ['Travel and Tourism'], 'start_date': '2016-07', 'end_date': '2018-04', 'job_location': 'Kuala Lumpur', 'job_duration': '1 year 9 months'}]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -600,38 +604,38 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Bachelor of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.98', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': 'N/A'}]</t>
+          <t>[{'field_of_study': 'Tourism Management', 'level': "Bachelor's Degree", 'cgpa': '3.38', 'university': 'TUNKU ABDUL RAHMAN UNIVERSITY COLLEGE', 'start_date': '2016', 'year_of_graduation': '2016'}, {'field_of_study': 'Hospitality Management', 'level': 'Diploma', 'cgpa': '3.20', 'university': 'N/A', 'start_date': '2014', 'year_of_graduation': '2014'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['Alteryx Designer Core Certified']</t>
+          <t>['Googe Analytics for Beginners', 'The Fundamental SQL Bootcamp', 'Python Programming for Beginners', 'Mastering SQL server']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Python', 'SQL', 'C++', 'R', 'Power BI', 'Tableau', 'Alteryx', 'Excel', 'Databricks', 'Azure Data Factory', 'Blob Storage', 'KeyVault', 'HTML', 'CSS', 'PHP', 'Bootstrap', 'JavaScript', 'C#', 'Cloud Foundation', 'Machine Learning', 'Data Analytic']</t>
+          <t>['Written and verbal communications in Chinese, English &amp; Malay', 'Familiar with airlines reservation system, Sabre &amp; Amadeus', 'Experienced with hotel distribution channels', 'Quick learner, ability to learn new skills quickly, act on feedback constructively and apply new knowledge immediately with the ability to identify learning opportunities']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['English', 'Malay', 'Chinese']</t>
+          <t>['Chinese', 'English', 'Malay']</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>2.8</v>
+        <v>7</v>
       </c>
       <c r="N2" t="n">
-        <v>6.9</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -655,7 +659,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t xml:space="preserve">N/A, </t>
+          <t xml:space="preserve">2016, 2014, </t>
         </is>
       </c>
       <c r="X2" t="n">
@@ -667,19 +671,29 @@
       <c r="Z2" t="inlineStr">
         <is>
           <t>**Alignments:**
-- The candidate holds a Bachelor's Degree in Computer Science with a focus on Data Engineering, which aligns with the educational background required for the job.
-- The candidate has skills in Python, SQL, Power BI, Tableau, Alteryx, and other relevant tools and technologies mentioned in the job requirements.
-- The candidate has professional certification in Alteryx, which is a plus as Alteryx is mentioned in the job requirements.
-- The candidate is proficient in English, Malay, and Chinese languages, which can be beneficial for communication in a diverse work environment.
+1. **Education Background:**
+   - The candidate has a Bachelor's Degree in Tourism Management and a Diploma in Hospitality Management, which aligns with the job description's requirement for a background in Tourism or Hospitality.
+2. **Skills:**
+   - The candidate has experience with airlines reservation systems like Sabre &amp; Amadeus, which aligns with the job requirement for familiarity with reservation systems.
+   - The candidate is proficient in written and verbal communications in Chinese, English, and Malay, which aligns with the job requirement for multilingual communication skills.
+3. **Previous Job Roles:**
+   - The candidate has held various roles in the Travel and Tourism industry, including Senior Corporate Travel Consultant positions, which align with the job description's requirement for relevant industry experience.
+4. **Professional Certificates:**
+   - The candidate has professional certificates in Google Analytics, SQL, and Python programming, which may align with the job requirement for technical skills or certifications.
 **Misalignments:**
-- The candidate's previous job roles as a PHP Web Developer and PPG Intern do not directly align with the job description for a Data Engineer.
-- The candidate's previous job roles do not demonstrate direct experience in data engineering or related fields.
-- The candidate's previous job roles do not show experience with the specific tools and technologies mentioned in the job requirements, such as Azure Data Factory, Blob Storage, and Databricks.
-- The candidate's previous job roles do not indicate experience with machine learning or data analytics, which are mentioned in the job requirements.</t>
+1. **Education Background:**
+   - The candidate's CGPA for the Bachelor's Degree and Diploma is not mentioned in the provided information, which could be a misalignment if the job description requires a specific GPA.
+2. **Skills:**
+   - While the candidate mentions being a quick learner and adaptable, specific skills or experiences related to the job description may not be explicitly mentioned.
+3. **Previous Job Roles:**
+   - The candidate's previous job roles focus on travel consultancy, but specific experience or achievements related to the job description's requirements may not be highlighted.
+4. **Professional Certificates:**
+   - The relevance of the professional certificates to the job description's requirements is not explicitly stated, so there may be a misalignment in terms of specific certification needs.
+Overall, the candidate's background in Tourism and Hospitality, relevant industry experience, and language skills align well with the job description. However, more explicit details on certain skills and experiences related to the job requirements could further strengthen the alignment.</t>
         </is>
       </c>
       <c r="AA2" t="n">
-        <v>28.7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update session_state seperated folder for each session
</commit_message>
<xml_diff>
--- a/post_criteria_evaluation.xlsx
+++ b/post_criteria_evaluation.xlsx
@@ -573,15 +573,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RUTH PONNIAH</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>60132969607</v>
+          <t>Mark Yean Tuck Ming</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+6012-225 1051</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ruthponniah96@yahoo.com</t>
+          <t>yeanmark@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -592,48 +594,48 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'RESEARCH AND DEVELOPMENT CHEMIST', 'job_company': 'Top Glove Int Sdn Bhd', 'Industries': ['Manufacturing', 'Textiles', 'Apparel', 'Leather and Footwear'], 'start_date': '2021-03', 'end_date': 'Present', 'job_location': 'Klang, Malaysia', 'job_duration': 'N/A'}, {'job_title': 'RESEARCH AND DEVELOPMENT INTERN', 'job_company': 'British American Tobacco', 'Industries': ['Tobacco'], 'start_date': '2018-09', 'end_date': '2019-08', 'job_location': 'Southampton, UK', 'job_duration': 'N/A'}, {'job_title': 'PRODUCTION CHEMISTRY INTERN', 'job_company': 'Petronas CariGali Sdn Bhd', 'Industries': ['Oil and Gas', 'Petrochemicals', 'Refining', 'Retail', 'Shipping', 'Exploration and Production', 'Engineering and Construction'], 'start_date': '2018-07', 'end_date': '2018-08', 'job_location': 'Sabah, Malaysia', 'job_duration': 'N/A'}]</t>
+          <t>[{'job_title': 'Data Engineer', 'job_company': 'CelcomDigi Sdn Bhd', 'Industries': ['Telecommunications'], 'start_date': '2022-05', 'end_date': '2023-05', 'job_location': 'N/A', 'job_duration': '1.0'}, {'job_title': 'Data Analyst Intern', 'job_company': 'MC Crenergy Sdn Bhd', 'Industries': ['Unknown'], 'start_date': '2019-11', 'end_date': '2020-03', 'job_location': 'N/A', 'job_duration': '0.3'}]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{'Country': 'Malaysia', 'State': 'Selangor', 'City': 'Shah Alam'}]</t>
+          <t>[{'Country': 'Malaysia', 'State': 'Selangor', 'City': 'Puchong'}]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'CHEMISTRY', 'level': 'Bachelor of Science + Master of Science', 'cgpa': '1st Class (Honors)', 'university': 'Queen’s University Belfast', 'start_date': '2015', 'year_of_graduation': '2020'}]</t>
+          <t>[{'field_of_study': 'Intelligence System', 'level': 'Bachelor Degree', 'cgpa': 'N/A', 'university': 'Asia Pacific University', 'start_date': '2018-02', 'year_of_graduation': '2021'}, {'field_of_study': 'Information Technology', 'level': 'Foundation', 'cgpa': 'N/A', 'university': 'Asia Pacific University', 'start_date': '2017-02', 'year_of_graduation': '2017'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['N/A']</t>
+          <t>['Project Management Workshop Series', 'Body Language Secrets: Nonverbal Communication Strategies', 'Computer Hacking Forensic Investigator', 'Certified Ethical Hacking Ver. 10', 'APIIT Certified Security Professional', 'Premier-Pride Challenge 2019', 'Artificial Intelligence Modules', 'AI and Machine Learning Competence for Industry 4.0', 'Certified Engineer in Computer Vision', 'Dataiku Core Designer Certificate']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['GMP Experience', 'Standard Laboratory Procedures including Synthetic and Analytical labs', 'Knowledgeable with COSHH requirements', 'Microsoft Office (Excel, PowerPoint, Outlook, Word)', 'Bruker NMR Spectroscopy Software (TopSpin) and ChemDraw', 'Minitab Statistical Software']</t>
+          <t>['Python', 'Selenium', 'BeautifulSoup', 'Pandas', 'Numpy', 'Matplotlib', 'Seaborn', 'Plotly', 'Supervised ML models', 'Unsupervised ML models', 'Natural Language Process', 'Computer Vision', 'Flask', 'DJango', 'Dash', 'MySQL', 'Teradata SQL', 'Oracle Data Integrator', 'Linux', 'C++', 'C#', 'Java', 'Microsoft Power BI', 'OLAP Cube', 'SSIS', 'ASP .net', 'DevExpress']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['English', 'Bahasa Malaysia', 'Mandarin']</t>
+          <t>['Chinese(Mandarin)', 'Chinese(Cantonese)', 'English', 'Malay']</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="N2" t="n">
-        <v>0.45</v>
+        <v>6.83</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -645,7 +647,7 @@
         <v>5</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -669,19 +671,21 @@
       <c r="Z2" t="inlineStr">
         <is>
           <t>**Alignments:**
-1. The candidate has a strong educational background in Chemistry with a Bachelor of Science and Master of Science from Queen’s University Belfast, aligning with the job requirement for a Chemistry-related field of study.
-2. The candidate has experience in GMP (Good Manufacturing Practices) from their previous job as a Research and Development Chemist, which aligns with the job requirement for GMP experience.
-3. The candidate is knowledgeable in Standard Laboratory Procedures, Synthetic and Analytical labs, and COSHH requirements, which align with the job requirement for laboratory skills.
-4. The candidate has experience with Bruker NMR Spectroscopy Software (TopSpin) and ChemDraw, aligning with the job requirement for specific software knowledge.
-5. The candidate has experience working in the Manufacturing industry as a Research and Development Chemist, aligning with the job requirement for experience in a related industry.
+1. **Education Background:** The candidate has a Bachelor's degree in Intelligence System, which aligns with the job description that may require a relevant educational background.
+2. **Skills:** The candidate possesses a wide range of technical skills such as Python, Selenium, Pandas, Numpy, etc., which align with the technical skills mentioned in the job requirements.
+3. **Previous Job Roles:** The candidate has experience as a Data Engineer and Data Analyst Intern, which aligns with the job description that may require experience in similar roles.
+4. **Professional Certificates:** The candidate holds certificates related to Project Management, Artificial Intelligence, and Machine Learning, which align with the job requirements that may require relevant certifications.
+5. **Languages:** The candidate is proficient in English, which aligns with the job requirements that may require proficiency in English.
 **Misalignments:**
-1. The candidate's previous job roles do not directly align with the job description provided, as the job description is not specified.
-2. The candidate does not have any listed professional certificates, which may be a requirement for the job.
-3. The candidate's language skills in English, Bahasa Malaysia, and Mandarin may not be directly relevant to the job unless specified in the job requirements.</t>
+1. **Education Background:** The candidate's foundation in Information Technology may not directly align with the job description's requirement for a specific field of study.
+2. **Skills:** While the candidate has a diverse set of technical skills, some of the skills mentioned may not be directly relevant to the job requirements, such as C++, C#, and ASP .net.
+3. **Previous Job Roles:** The candidate's previous job roles are in the Telecommunications and Unknown industries, which may not directly align with the industry or domain specified in the job description.
+4. **Professional Certificates:** Some of the certificates held by the candidate, such as Body Language Secrets and Certified Ethical Hacking, may not directly align with the job requirements unless explicitly mentioned in the job description.
+5. **Languages:** The candidate's proficiency in Chinese (Mandarin and Cantonese) and Malay may not be directly relevant to the job requirements unless specified in the job description.</t>
         </is>
       </c>
       <c r="AA2" t="n">
-        <v>9.25</v>
+        <v>28.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>